<commit_message>
committed on 26 june
</commit_message>
<xml_diff>
--- a/testData/Opencart_data.xlsx
+++ b/testData/Opencart_data.xlsx
@@ -1,22 +1,17 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" mc:Ignorable="x15">
-  <fileVersion appName="xl" lastEdited="6" lowestEdited="6" rupBuild="14420"/>
-  <workbookPr defaultThemeVersion="164011"/>
-  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
-    <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\nigin.john\AppData\Local\Microsoft\Windows\INetCache\Content.Outlook\72TXEVPY\"/>
-    </mc:Choice>
-  </mc:AlternateContent>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+  <fileVersion appName="xl" lastEdited="4" lowestEdited="6" rupBuild="4505"/>
+  <workbookPr/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="28800" windowHeight="12300"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="20730" windowHeight="11760"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
   </sheets>
-  <calcPr calcId="162913"/>
-  <extLst>
-    <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
+  <calcPr calcId="124519"/>
+  <extLst xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main">
+    <ext uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
       <x15:workbookPr chartTrackingRefBase="1"/>
     </ext>
   </extLst>
@@ -24,44 +19,26 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="21" uniqueCount="17">
-  <si>
-    <t>test0619a@gmail.com</t>
-  </si>
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="21" uniqueCount="16">
   <si>
     <t>pavanoltraining@gmail.com</t>
   </si>
   <si>
-    <t>lakshmi@yahoo.com</t>
-  </si>
-  <si>
     <t>laksh@yahoo.com</t>
   </si>
   <si>
     <t>laks@yahoo.com</t>
   </si>
   <si>
-    <t>mtest0619@gmail.com</t>
-  </si>
-  <si>
-    <t>Test@0619</t>
-  </si>
-  <si>
     <t>Lakshmi</t>
   </si>
   <si>
     <t>test@123</t>
   </si>
   <si>
-    <t>Laxmi</t>
-  </si>
-  <si>
     <t>xyz</t>
   </si>
   <si>
-    <t>Mtest@0619</t>
-  </si>
-  <si>
     <t>Valid</t>
   </si>
   <si>
@@ -75,13 +52,28 @@
   </si>
   <si>
     <t>res</t>
+  </si>
+  <si>
+    <t>mtest0626@gmail.com</t>
+  </si>
+  <si>
+    <t>Mtest@0623</t>
+  </si>
+  <si>
+    <t>mtest0626b@gmail.com</t>
+  </si>
+  <si>
+    <t>mtest0626c@gmail.com</t>
+  </si>
+  <si>
+    <t>Mtest@0626</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" mc:Ignorable="x14ac x16r2">
-  <fonts count="2" x14ac:knownFonts="1">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
+  <fonts count="3">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -96,6 +88,13 @@
       <name val="Calibri"/>
       <family val="2"/>
       <scheme val="minor"/>
+    </font>
+    <font>
+      <u/>
+      <sz val="11"/>
+      <color theme="10"/>
+      <name val="Calibri"/>
+      <family val="2"/>
     </font>
   </fonts>
   <fills count="3">
@@ -136,10 +135,14 @@
       <diagonal/>
     </border>
   </borders>
-  <cellStyleXfs count="1">
+  <cellStyleXfs count="2">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="top"/>
+      <protection locked="0"/>
+    </xf>
   </cellStyleXfs>
-  <cellXfs count="3">
+  <cellXfs count="4">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
@@ -147,8 +150,12 @@
     <xf numFmtId="0" fontId="1" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="1" xfId="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment horizontal="center"/>
+    </xf>
   </cellXfs>
-  <cellStyles count="1">
+  <cellStyles count="2">
+    <cellStyle name="Hyperlink" xfId="1" builtinId="8"/>
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
   <dxfs count="0"/>
@@ -207,7 +214,7 @@
     </a:clrScheme>
     <a:fontScheme name="Office">
       <a:majorFont>
-        <a:latin typeface="Calibri Light" panose="020F0302020204030204"/>
+        <a:latin typeface="Calibri Light"/>
         <a:ea typeface=""/>
         <a:cs typeface=""/>
         <a:font script="Jpan" typeface="游ゴシック Light"/>
@@ -242,7 +249,7 @@
         <a:font script="Geor" typeface="Sylfaen"/>
       </a:majorFont>
       <a:minorFont>
-        <a:latin typeface="Calibri" panose="020F0502020204030204"/>
+        <a:latin typeface="Calibri"/>
         <a:ea typeface=""/>
         <a:cs typeface=""/>
         <a:font script="Jpan" typeface="游ゴシック"/>
@@ -419,104 +426,112 @@
   <a:extraClrSchemeLst/>
   <a:extLst>
     <a:ext uri="{05A4C25C-085E-4340-85A3-A5531E510DB2}">
-      <thm15:themeFamily xmlns:thm15="http://schemas.microsoft.com/office/thememl/2012/main" name="Office Theme" id="{62F939B6-93AF-4DB8-9C6B-D6C7DFDC589F}" vid="{4A3C46E8-61CC-4603-A589-7422A47A8E4A}"/>
+      <thm15:themeFamily xmlns:thm15="http://schemas.microsoft.com/office/thememl/2012/main" xmlns="" name="Office Theme" id="{62F939B6-93AF-4DB8-9C6B-D6C7DFDC589F}" vid="{4A3C46E8-61CC-4603-A589-7422A47A8E4A}"/>
     </a:ext>
   </a:extLst>
 </a:theme>
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
   <dimension ref="A1:C7"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="E5" sqref="E5"/>
+      <selection activeCell="C12" sqref="C12"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultRowHeight="15"/>
   <cols>
     <col min="1" max="1" width="26.42578125" bestFit="1" customWidth="1"/>
     <col min="2" max="2" width="12" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:3">
       <c r="A1" s="2" t="s">
+        <v>8</v>
+      </c>
+      <c r="B1" s="2" t="s">
+        <v>9</v>
+      </c>
+      <c r="C1" s="2" t="s">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="2" spans="1:3">
+      <c r="A2" s="3" t="s">
+        <v>11</v>
+      </c>
+      <c r="B2" s="3" t="s">
+        <v>12</v>
+      </c>
+      <c r="C2" s="1" t="s">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="3" spans="1:3">
+      <c r="A3" s="1" t="s">
+        <v>0</v>
+      </c>
+      <c r="B3" s="1" t="s">
+        <v>4</v>
+      </c>
+      <c r="C3" s="1" t="s">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="4" spans="1:3">
+      <c r="A4" s="3" t="s">
+        <v>13</v>
+      </c>
+      <c r="B4" s="3" t="s">
+        <v>12</v>
+      </c>
+      <c r="C4" s="1" t="s">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="5" spans="1:3">
+      <c r="A5" s="1" t="s">
+        <v>1</v>
+      </c>
+      <c r="B5" s="1" t="s">
+        <v>3</v>
+      </c>
+      <c r="C5" s="1" t="s">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="6" spans="1:3">
+      <c r="A6" s="1" t="s">
+        <v>2</v>
+      </c>
+      <c r="B6" s="1" t="s">
+        <v>5</v>
+      </c>
+      <c r="C6" s="1" t="s">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="7" spans="1:3">
+      <c r="A7" s="3" t="s">
         <v>14</v>
       </c>
-      <c r="B1" s="2" t="s">
+      <c r="B7" s="3" t="s">
         <v>15</v>
       </c>
-      <c r="C1" s="2" t="s">
-        <v>16</v>
-      </c>
-    </row>
-    <row r="2" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A2" s="1" t="s">
-        <v>0</v>
-      </c>
-      <c r="B2" s="1" t="s">
+      <c r="C7" s="1" t="s">
         <v>6</v>
       </c>
-      <c r="C2" s="1" t="s">
-        <v>12</v>
-      </c>
-    </row>
-    <row r="3" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A3" s="1" t="s">
-        <v>1</v>
-      </c>
-      <c r="B3" s="1" t="s">
-        <v>8</v>
-      </c>
-      <c r="C3" s="1" t="s">
-        <v>13</v>
-      </c>
-    </row>
-    <row r="4" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A4" s="1" t="s">
-        <v>2</v>
-      </c>
-      <c r="B4" s="1" t="s">
-        <v>9</v>
-      </c>
-      <c r="C4" s="1" t="s">
-        <v>13</v>
-      </c>
-    </row>
-    <row r="5" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A5" s="1" t="s">
-        <v>3</v>
-      </c>
-      <c r="B5" s="1" t="s">
-        <v>7</v>
-      </c>
-      <c r="C5" s="1" t="s">
-        <v>13</v>
-      </c>
-    </row>
-    <row r="6" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A6" s="1" t="s">
-        <v>4</v>
-      </c>
-      <c r="B6" s="1" t="s">
-        <v>10</v>
-      </c>
-      <c r="C6" s="1" t="s">
-        <v>13</v>
-      </c>
-    </row>
-    <row r="7" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A7" s="1" t="s">
-        <v>5</v>
-      </c>
-      <c r="B7" s="1" t="s">
-        <v>11</v>
-      </c>
-      <c r="C7" s="1" t="s">
-        <v>12</v>
-      </c>
     </row>
   </sheetData>
+  <hyperlinks>
+    <hyperlink ref="A2" r:id="rId1"/>
+    <hyperlink ref="B2" r:id="rId2"/>
+    <hyperlink ref="A4" r:id="rId3"/>
+    <hyperlink ref="B4" r:id="rId4"/>
+    <hyperlink ref="A7" r:id="rId5"/>
+    <hyperlink ref="B7" r:id="rId6"/>
+  </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
 </file>
</xml_diff>